<commit_message>
[service] add appointment feature
</commit_message>
<xml_diff>
--- a/src/main/resources/db/weshare_data_design.xlsx
+++ b/src/main/resources/db/weshare_data_design.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiding/Documents/WolferX/wolferspring/src/main/resources/db/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="14280" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t>user</t>
   </si>
@@ -165,12 +173,6 @@
     <t>refresh_token</t>
   </si>
   <si>
-    <t>user_a_id (FK)</t>
-  </si>
-  <si>
-    <t>user_b_id (FK)</t>
-  </si>
-  <si>
     <t>phone_rate</t>
   </si>
   <si>
@@ -214,6 +216,45 @@
   </si>
   <si>
     <t>like_type</t>
+  </si>
+  <si>
+    <t>user_a_id (FK,PK)</t>
+  </si>
+  <si>
+    <t>user_b_id (FK,PK)</t>
+  </si>
+  <si>
+    <t>schema_version</t>
+  </si>
+  <si>
+    <t>installed_rank(PK)</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>checksum</t>
+  </si>
+  <si>
+    <t>installed_by</t>
+  </si>
+  <si>
+    <t>installed_on</t>
+  </si>
+  <si>
+    <t>execution_time</t>
+  </si>
+  <si>
+    <t>success</t>
   </si>
 </sst>
 </file>
@@ -471,6 +512,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -799,10 +845,10 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
@@ -814,7 +860,7 @@
     <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -830,10 +876,13 @@
       <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -849,10 +898,13 @@
       <c r="E2" t="s">
         <v>34</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -868,10 +920,13 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -887,10 +942,13 @@
       <c r="E4" t="s">
         <v>32</v>
       </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -901,15 +959,18 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
@@ -920,15 +981,18 @@
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
@@ -944,10 +1008,13 @@
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -963,10 +1030,13 @@
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -980,10 +1050,13 @@
         <v>11</v>
       </c>
       <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -992,12 +1065,15 @@
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1006,12 +1082,15 @@
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1019,7 +1098,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>44</v>
       </c>
@@ -1027,7 +1106,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1035,7 +1114,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>43</v>
@@ -1044,7 +1123,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -1052,58 +1131,58 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -1112,15 +1191,15 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>10</v>
@@ -1129,15 +1208,15 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>11</v>
@@ -1146,9 +1225,9 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -1157,7 +1236,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
         <v>16</v>
@@ -1169,7 +1248,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -1177,17 +1256,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
@@ -1195,10 +1274,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>